<commit_message>
added intended use field
</commit_message>
<xml_diff>
--- a/datasets/Campylobacter_jejuni_0810PADBR-1.xlsx
+++ b/datasets/Campylobacter_jejuni_0810PADBR-1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="137">
   <si>
     <t>Organism</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>e540eb31585ef307e29c615d6dab6d1da1f21f0f886355cb5a526a0a10d31895</t>
+  </si>
+  <si>
+    <t>intendedUse</t>
+  </si>
+  <si>
+    <t>Epi-validated outbreak</t>
   </si>
 </sst>
 </file>
@@ -489,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -503,6 +509,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,11 +863,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -919,82 +926,61 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="s">
-        <v>91</v>
-      </c>
-      <c r="J9" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
@@ -1003,27 +989,24 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
-      </c>
-      <c r="K10" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>3</v>
@@ -1032,13 +1015,13 @@
         <v>3</v>
       </c>
       <c r="G11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K11" t="s">
         <v>90</v>
@@ -1046,16 +1029,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
@@ -1064,13 +1047,13 @@
         <v>3</v>
       </c>
       <c r="G12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K12" t="s">
         <v>90</v>
@@ -1078,16 +1061,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -1099,10 +1082,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K13" t="s">
         <v>90</v>
@@ -1110,16 +1093,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
         <v>3</v>
@@ -1131,10 +1114,10 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K14" t="s">
         <v>90</v>
@@ -1142,16 +1125,16 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
         <v>3</v>
@@ -1163,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K15" t="s">
         <v>90</v>
@@ -1174,16 +1157,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
@@ -1195,27 +1178,27 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
         <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
@@ -1227,27 +1210,27 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
         <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
@@ -1259,10 +1242,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K18" t="s">
         <v>90</v>
@@ -1270,16 +1253,16 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
         <v>3</v>
@@ -1291,10 +1274,10 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K19" t="s">
         <v>90</v>
@@ -1302,16 +1285,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
         <v>3</v>
@@ -1323,27 +1306,27 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E21" t="s">
         <v>3</v>
@@ -1355,27 +1338,27 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
         <v>3</v>
@@ -1387,10 +1370,10 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K22" t="s">
         <v>90</v>
@@ -1398,16 +1381,16 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
         <v>3</v>
@@ -1419,10 +1402,10 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K23" t="s">
         <v>90</v>
@@ -1430,19 +1413,19 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>69</v>
+      <c r="D24" t="s">
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
         <v>3</v>
@@ -1451,24 +1434,27 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J24" t="s">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="K24" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
         <v>24</v>
@@ -1480,24 +1466,24 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
         <v>22</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
         <v>24</v>
@@ -1509,27 +1495,27 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
         <v>22</v>
       </c>
-      <c r="D27" t="s">
-        <v>78</v>
+      <c r="D27" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="F27" t="s">
         <v>3</v>
@@ -1538,24 +1524,24 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
         <v>79</v>
@@ -1567,27 +1553,27 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>110</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>132</v>
+        <v>109</v>
+      </c>
+      <c r="J28" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
         <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
         <v>3</v>
@@ -1596,38 +1582,67 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>111</v>
-      </c>
-      <c r="J29" t="s">
-        <v>133</v>
+        <v>110</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>111</v>
+      </c>
+      <c r="J30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>86</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>87</v>
       </c>
-      <c r="C30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
         <v>88</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>79</v>
       </c>
-      <c r="F30" t="s">
-        <v>3</v>
-      </c>
-      <c r="G30" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
         <v>112</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J31" t="s">
         <v>134</v>
       </c>
     </row>

</xml_diff>